<commit_message>
update ceph luminous owncloud 10
</commit_message>
<xml_diff>
--- a/Lab/PIC/IP-Planning-Hardware-Requirements.xlsx
+++ b/Lab/PIC/IP-Planning-Hardware-Requirements.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitRepo\khoa-luan\Lab\PIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="12795" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27825" windowHeight="12795" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CEPH-Alone" sheetId="7" r:id="rId1"/>
     <sheet name="OpenStack_Ceph-AIO-Ubuntu" sheetId="8" r:id="rId2"/>
     <sheet name="OpenStack_Ceph-AIO-CentOS" sheetId="9" r:id="rId3"/>
-    <sheet name="OpenStack_Pike" sheetId="10" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId5"/>
+    <sheet name="jewel-nextcloud" sheetId="10" r:id="rId4"/>
+    <sheet name="luminous" sheetId="11" r:id="rId5"/>
+    <sheet name="luminous-owncloud" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="73">
   <si>
     <t>Controller</t>
   </si>
@@ -248,6 +249,13 @@
   </si>
   <si>
     <t>IP PLANNING - Ceph Luminous 3 Node</t>
+  </si>
+  <si>
+    <t>ceph-client
+owncloud</t>
+  </si>
+  <si>
+    <t>IP PLANNING - Ceph Luminous with Owncloud</t>
   </si>
 </sst>
 </file>
@@ -621,6 +629,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,12 +641,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -654,7 +665,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -666,19 +683,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -688,27 +696,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -719,6 +706,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,23 +1027,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="52"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -1079,7 +1087,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1093,30 +1101,30 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="52">
-        <v>4</v>
-      </c>
-      <c r="I4" s="52">
+      <c r="H4" s="45">
+        <v>4</v>
+      </c>
+      <c r="I4" s="45">
         <v>2</v>
       </c>
-      <c r="J4" s="44">
+      <c r="J4" s="46">
         <v>40</v>
       </c>
-      <c r="K4" s="45">
+      <c r="K4" s="41">
         <v>60</v>
       </c>
-      <c r="L4" s="45">
+      <c r="L4" s="41">
         <v>60</v>
       </c>
-      <c r="M4" s="45">
+      <c r="M4" s="41">
         <v>60</v>
       </c>
-      <c r="N4" s="45">
+      <c r="N4" s="41">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="42"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1132,16 +1140,16 @@
       <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1153,16 +1161,16 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1170,16 +1178,16 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1193,30 +1201,30 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="52">
-        <v>4</v>
-      </c>
-      <c r="I8" s="52">
+      <c r="H8" s="45">
+        <v>4</v>
+      </c>
+      <c r="I8" s="45">
         <v>2</v>
       </c>
-      <c r="J8" s="44">
+      <c r="J8" s="46">
         <v>40</v>
       </c>
-      <c r="K8" s="45">
+      <c r="K8" s="41">
         <v>60</v>
       </c>
-      <c r="L8" s="45">
+      <c r="L8" s="41">
         <v>60</v>
       </c>
-      <c r="M8" s="45">
+      <c r="M8" s="41">
         <v>60</v>
       </c>
-      <c r="N8" s="45">
+      <c r="N8" s="41">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1232,16 +1240,16 @@
       <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1253,16 +1261,16 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1270,16 +1278,16 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="42" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1293,30 +1301,30 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="52">
-        <v>4</v>
-      </c>
-      <c r="I12" s="52">
+      <c r="H12" s="45">
+        <v>4</v>
+      </c>
+      <c r="I12" s="45">
         <v>2</v>
       </c>
-      <c r="J12" s="44">
+      <c r="J12" s="46">
         <v>40</v>
       </c>
-      <c r="K12" s="45">
+      <c r="K12" s="41">
         <v>60</v>
       </c>
-      <c r="L12" s="45">
+      <c r="L12" s="41">
         <v>60</v>
       </c>
-      <c r="M12" s="45">
+      <c r="M12" s="41">
         <v>60</v>
       </c>
-      <c r="N12" s="45">
+      <c r="N12" s="41">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1332,16 +1340,16 @@
       <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="42"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1353,16 +1361,16 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="43"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1370,16 +1378,26 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
@@ -1396,16 +1414,6 @@
     <mergeCell ref="L8:L11"/>
     <mergeCell ref="M8:M11"/>
     <mergeCell ref="N8:N11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:N2"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1432,40 +1440,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="58"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1509,7 +1517,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="53" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1523,24 +1531,24 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="59">
+      <c r="H5" s="55">
         <v>6</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="45">
         <v>2</v>
       </c>
-      <c r="J5" s="44">
+      <c r="J5" s="46">
         <v>100</v>
       </c>
-      <c r="K5" s="45">
+      <c r="K5" s="41">
         <v>60</v>
       </c>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="57"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
@@ -1556,16 +1564,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="59"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1579,22 +1587,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="59">
+      <c r="H7" s="55">
         <v>8</v>
       </c>
-      <c r="I7" s="52">
-        <v>4</v>
-      </c>
-      <c r="J7" s="44">
+      <c r="I7" s="45">
+        <v>4</v>
+      </c>
+      <c r="J7" s="46">
         <v>100</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="57"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
@@ -1610,16 +1618,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="59"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="53" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1633,22 +1641,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="59">
+      <c r="H9" s="55">
         <v>8</v>
       </c>
-      <c r="I9" s="52">
-        <v>4</v>
-      </c>
-      <c r="J9" s="44">
+      <c r="I9" s="45">
+        <v>4</v>
+      </c>
+      <c r="J9" s="46">
         <v>60</v>
       </c>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="14" t="s">
         <v>2</v>
       </c>
@@ -1664,16 +1672,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -1687,30 +1695,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="59">
+      <c r="H11" s="55">
         <v>8</v>
       </c>
-      <c r="I11" s="52">
-        <v>4</v>
-      </c>
-      <c r="J11" s="44">
+      <c r="I11" s="45">
+        <v>4</v>
+      </c>
+      <c r="J11" s="46">
         <v>60</v>
       </c>
-      <c r="K11" s="45">
+      <c r="K11" s="41">
         <v>50</v>
       </c>
-      <c r="L11" s="45">
+      <c r="L11" s="41">
         <v>50</v>
       </c>
-      <c r="M11" s="45">
+      <c r="M11" s="41">
         <v>50</v>
       </c>
-      <c r="N11" s="45">
+      <c r="N11" s="41">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="57"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="15" t="s">
         <v>2</v>
       </c>
@@ -1726,16 +1734,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="59"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="14" t="s">
         <v>23</v>
       </c>
@@ -1747,35 +1755,16 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
     <mergeCell ref="B2:N2"/>
@@ -1792,6 +1781,25 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1820,40 +1828,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="58"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1897,7 +1905,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="53" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="26" t="s">
@@ -1911,24 +1919,24 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="59">
+      <c r="H5" s="55">
         <v>6</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="45">
         <v>2</v>
       </c>
-      <c r="J5" s="44">
+      <c r="J5" s="46">
         <v>100</v>
       </c>
-      <c r="K5" s="45">
+      <c r="K5" s="41">
         <v>60</v>
       </c>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="57"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="27" t="s">
         <v>47</v>
       </c>
@@ -1944,16 +1952,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="59"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -1967,22 +1975,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="59">
+      <c r="H7" s="55">
         <v>8</v>
       </c>
-      <c r="I7" s="52">
-        <v>4</v>
-      </c>
-      <c r="J7" s="44">
+      <c r="I7" s="45">
+        <v>4</v>
+      </c>
+      <c r="J7" s="46">
         <v>100</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="57"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="27" t="s">
         <v>40</v>
       </c>
@@ -1998,16 +2006,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="59"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="53" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="28" t="s">
@@ -2021,22 +2029,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="59">
+      <c r="H9" s="55">
         <v>8</v>
       </c>
-      <c r="I9" s="52">
-        <v>4</v>
-      </c>
-      <c r="J9" s="44">
+      <c r="I9" s="45">
+        <v>4</v>
+      </c>
+      <c r="J9" s="46">
         <v>60</v>
       </c>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="27" t="s">
         <v>40</v>
       </c>
@@ -2052,16 +2060,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -2075,30 +2083,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="59">
+      <c r="H11" s="55">
         <v>8</v>
       </c>
-      <c r="I11" s="52">
-        <v>4</v>
-      </c>
-      <c r="J11" s="44">
+      <c r="I11" s="45">
+        <v>4</v>
+      </c>
+      <c r="J11" s="46">
         <v>60</v>
       </c>
-      <c r="K11" s="45">
+      <c r="K11" s="41">
         <v>50</v>
       </c>
-      <c r="L11" s="45">
+      <c r="L11" s="41">
         <v>50</v>
       </c>
-      <c r="M11" s="45">
+      <c r="M11" s="41">
         <v>50</v>
       </c>
-      <c r="N11" s="45">
+      <c r="N11" s="41">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="57"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="29" t="s">
         <v>40</v>
       </c>
@@ -2114,16 +2122,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="59"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="30" t="s">
         <v>41</v>
       </c>
@@ -2135,16 +2143,37 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
@@ -2159,27 +2188,6 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2190,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2209,42 +2217,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="55"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="58"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="49" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
     </row>
     <row r="4" spans="2:15" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -2291,7 +2299,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="26" t="s">
@@ -2312,22 +2320,22 @@
       <c r="H5" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="65">
+      <c r="I5" s="67">
         <v>2</v>
       </c>
-      <c r="J5" s="65">
+      <c r="J5" s="67">
         <v>2</v>
       </c>
       <c r="K5" s="62">
         <v>50</v>
       </c>
-      <c r="L5" s="60"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
     </row>
     <row r="6" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="29" t="s">
         <v>49</v>
       </c>
@@ -2342,32 +2350,32 @@
       </c>
       <c r="G6" s="29"/>
       <c r="H6" s="37"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
       <c r="K6" s="63"/>
-      <c r="L6" s="69"/>
+      <c r="L6" s="72"/>
       <c r="M6" s="61"/>
       <c r="N6" s="61"/>
       <c r="O6" s="61"/>
     </row>
     <row r="7" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="35"/>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
       <c r="H7" s="38"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="70"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="73"/>
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
     </row>
     <row r="8" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="26" t="s">
@@ -2388,24 +2396,24 @@
       <c r="H8" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="65">
+      <c r="I8" s="67">
         <v>2</v>
       </c>
-      <c r="J8" s="65">
+      <c r="J8" s="67">
         <v>2</v>
       </c>
       <c r="K8" s="62">
         <v>50</v>
       </c>
-      <c r="L8" s="60" t="s">
+      <c r="L8" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
     </row>
     <row r="9" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="29" t="s">
         <v>49</v>
       </c>
@@ -2420,32 +2428,32 @@
       </c>
       <c r="G9" s="29"/>
       <c r="H9" s="37"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
       <c r="K9" s="63"/>
-      <c r="L9" s="69"/>
+      <c r="L9" s="72"/>
       <c r="M9" s="61"/>
       <c r="N9" s="61"/>
       <c r="O9" s="61"/>
     </row>
     <row r="10" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
       <c r="E10" s="35"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
       <c r="H10" s="38"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
       <c r="K10" s="32"/>
-      <c r="L10" s="70"/>
+      <c r="L10" s="73"/>
       <c r="M10" s="33"/>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
     </row>
     <row r="11" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="42" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="26" t="s">
@@ -2466,24 +2474,24 @@
       <c r="H11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="65">
+      <c r="I11" s="67">
         <v>2</v>
       </c>
-      <c r="J11" s="65">
+      <c r="J11" s="67">
         <v>2</v>
       </c>
       <c r="K11" s="62">
         <v>50</v>
       </c>
-      <c r="L11" s="60" t="s">
+      <c r="L11" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
     </row>
     <row r="12" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="29" t="s">
         <v>49</v>
       </c>
@@ -2498,32 +2506,32 @@
       </c>
       <c r="G12" s="29"/>
       <c r="H12" s="37"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
       <c r="K12" s="63"/>
-      <c r="L12" s="69"/>
+      <c r="L12" s="72"/>
       <c r="M12" s="61"/>
       <c r="N12" s="61"/>
       <c r="O12" s="61"/>
     </row>
     <row r="13" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="35"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="38"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="70"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="73"/>
       <c r="M13" s="33"/>
       <c r="N13" s="33"/>
       <c r="O13" s="33"/>
     </row>
     <row r="14" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="64" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="26" t="s">
@@ -2544,22 +2552,22 @@
       <c r="H14" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="65">
+      <c r="I14" s="67">
         <v>2</v>
       </c>
-      <c r="J14" s="65">
+      <c r="J14" s="67">
         <v>2</v>
       </c>
       <c r="K14" s="62">
         <v>50</v>
       </c>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="71"/>
     </row>
     <row r="15" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="72"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="29" t="s">
         <v>64</v>
       </c>
@@ -2578,32 +2586,56 @@
       <c r="H15" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
       <c r="K15" s="63"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
     </row>
     <row r="16" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="73"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="34"/>
       <c r="D16" s="30"/>
       <c r="E16" s="24"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="39"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="70"/>
-      <c r="M16" s="70"/>
-      <c r="N16" s="70"/>
-      <c r="O16" s="70"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="N14:N16"/>
+    <mergeCell ref="O14:O16"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L8:L10"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B3:H3"/>
@@ -2611,32 +2643,8 @@
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="O5:O6"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="K14:K16"/>
-    <mergeCell ref="L14:L16"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="N14:N16"/>
-    <mergeCell ref="O14:O16"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="J11:J13"/>
     <mergeCell ref="L5:L7"/>
     <mergeCell ref="K5:K7"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="L11:L13"/>
     <mergeCell ref="I5:I7"/>
     <mergeCell ref="J5:J7"/>
   </mergeCells>
@@ -2650,7 +2658,7 @@
   <dimension ref="B2:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2668,42 +2676,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="55"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="58"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="49" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
     </row>
     <row r="4" spans="2:15" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -2750,7 +2758,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="26" t="s">
@@ -2771,22 +2779,22 @@
       <c r="H5" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="65">
+      <c r="I5" s="67">
         <v>2</v>
       </c>
-      <c r="J5" s="65">
+      <c r="J5" s="67">
         <v>2</v>
       </c>
       <c r="K5" s="62">
         <v>50</v>
       </c>
-      <c r="L5" s="60"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
     </row>
     <row r="6" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="29" t="s">
         <v>49</v>
       </c>
@@ -2801,32 +2809,32 @@
       </c>
       <c r="G6" s="29"/>
       <c r="H6" s="37"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
       <c r="K6" s="63"/>
-      <c r="L6" s="69"/>
+      <c r="L6" s="72"/>
       <c r="M6" s="61"/>
       <c r="N6" s="61"/>
       <c r="O6" s="61"/>
     </row>
     <row r="7" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="35"/>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
       <c r="H7" s="38"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="70"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="73"/>
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
     </row>
     <row r="8" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="26" t="s">
@@ -2847,24 +2855,24 @@
       <c r="H8" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="65">
+      <c r="I8" s="67">
         <v>2</v>
       </c>
-      <c r="J8" s="65">
+      <c r="J8" s="67">
         <v>2</v>
       </c>
       <c r="K8" s="62">
         <v>50</v>
       </c>
-      <c r="L8" s="60" t="s">
+      <c r="L8" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
     </row>
     <row r="9" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="29" t="s">
         <v>49</v>
       </c>
@@ -2879,32 +2887,32 @@
       </c>
       <c r="G9" s="29"/>
       <c r="H9" s="37"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
       <c r="K9" s="63"/>
-      <c r="L9" s="69"/>
+      <c r="L9" s="72"/>
       <c r="M9" s="61"/>
       <c r="N9" s="61"/>
       <c r="O9" s="61"/>
     </row>
     <row r="10" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
       <c r="E10" s="35"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
       <c r="H10" s="38"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
       <c r="K10" s="32"/>
-      <c r="L10" s="70"/>
+      <c r="L10" s="73"/>
       <c r="M10" s="33"/>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
     </row>
     <row r="11" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="42" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="26" t="s">
@@ -2925,24 +2933,24 @@
       <c r="H11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="65">
+      <c r="I11" s="67">
         <v>2</v>
       </c>
-      <c r="J11" s="65">
+      <c r="J11" s="67">
         <v>2</v>
       </c>
       <c r="K11" s="62">
         <v>50</v>
       </c>
-      <c r="L11" s="60" t="s">
+      <c r="L11" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
     </row>
     <row r="12" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="29" t="s">
         <v>49</v>
       </c>
@@ -2957,26 +2965,26 @@
       </c>
       <c r="G12" s="29"/>
       <c r="H12" s="37"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
       <c r="K12" s="63"/>
-      <c r="L12" s="69"/>
+      <c r="L12" s="72"/>
       <c r="M12" s="61"/>
       <c r="N12" s="61"/>
       <c r="O12" s="61"/>
     </row>
     <row r="13" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="35"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="38"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="70"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="73"/>
       <c r="M13" s="33"/>
       <c r="N13" s="33"/>
       <c r="O13" s="33"/>
@@ -3031,7 +3039,466 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
     <mergeCell ref="O11:O12"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C484A0-D3C8-4FE6-9413-8A568BE3FF19}">
+  <dimension ref="B2:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="40" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="31" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="58"/>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
+    </row>
+    <row r="4" spans="2:15" ht="33" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="67">
+        <v>2</v>
+      </c>
+      <c r="J5" s="67">
+        <v>2</v>
+      </c>
+      <c r="K5" s="62">
+        <v>50</v>
+      </c>
+      <c r="L5" s="71"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+    </row>
+    <row r="6" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="43"/>
+      <c r="C6" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+    </row>
+    <row r="7" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+    </row>
+    <row r="8" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="67">
+        <v>2</v>
+      </c>
+      <c r="J8" s="67">
+        <v>2</v>
+      </c>
+      <c r="K8" s="62">
+        <v>50</v>
+      </c>
+      <c r="L8" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+    </row>
+    <row r="9" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="43"/>
+      <c r="C9" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+    </row>
+    <row r="10" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+    </row>
+    <row r="11" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="67">
+        <v>2</v>
+      </c>
+      <c r="J11" s="67">
+        <v>2</v>
+      </c>
+      <c r="K11" s="62">
+        <v>50</v>
+      </c>
+      <c r="L11" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+    </row>
+    <row r="12" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="43"/>
+      <c r="C12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="29"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+    </row>
+    <row r="13" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="44"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+    </row>
+    <row r="14" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="67">
+        <v>2</v>
+      </c>
+      <c r="J14" s="67">
+        <v>2</v>
+      </c>
+      <c r="K14" s="62">
+        <v>50</v>
+      </c>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="71"/>
+    </row>
+    <row r="15" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="65"/>
+      <c r="C15" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
+    </row>
+    <row r="16" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="66"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="73"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="N14:N16"/>
+    <mergeCell ref="O14:O16"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
@@ -3057,7 +3524,6 @@
     <mergeCell ref="L5:L7"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N11:N12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>